<commit_message>
added final/gross energy consumption charts
</commit_message>
<xml_diff>
--- a/data/data_raw/eurostat/AT_2021_energy_balance_TWh.xlsx
+++ b/data/data_raw/eurostat/AT_2021_energy_balance_TWh.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernhard\Documents\EnergyAnalysis\Data\Dashboard\data\data_raw\eurostat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D10F3D9-F393-4BEC-B8A0-725CE936EE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF28715-BF31-4138-990E-410651ECE3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1020,21 +1033,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BU139"/>
+  <dimension ref="A1:BY139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BL88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A121" sqref="A121"/>
+      <selection pane="bottomRight" activeCell="BT96" sqref="BT96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="102.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="102.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="47.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1255,7 +1270,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1374,7 +1389,7 @@
         <v>21.16242611111111</v>
       </c>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1481,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1681,7 +1696,7 @@
         <v>238.62689750000001</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -1881,7 +1896,7 @@
         <v>37.877901944444439</v>
       </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -2072,7 +2087,7 @@
         <v>44.504066944444453</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -2293,7 +2308,7 @@
         <v>266.41548833333331</v>
       </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -2436,7 +2451,7 @@
         <v>0.22362361111111109</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -2657,7 +2672,7 @@
         <v>266.19186500000001</v>
       </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -2743,7 +2758,7 @@
         <v>4.6890772222222221</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -2964,7 +2979,7 @@
         <v>261.50278777777783</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -2972,7 +2987,7 @@
         <v>391.66603972222231</v>
       </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -2980,7 +2995,7 @@
         <v>366.94124583333343</v>
       </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -2988,7 +3003,7 @@
         <v>323.53252388888887</v>
       </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -3209,7 +3224,7 @@
         <v>178.86723555555551</v>
       </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -3430,7 +3445,7 @@
         <v>40.487499166666673</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -3633,7 +3648,7 @@
         <v>4.9399833333333332</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -3824,7 +3839,7 @@
         <v>17.23578805555556</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -4018,7 +4033,7 @@
         <v>2.920797777777778</v>
       </c>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -4221,7 +4236,7 @@
         <v>8.9668227777777787</v>
       </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -4412,7 +4427,7 @@
         <v>5.2079322222222224</v>
       </c>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -4606,7 +4621,7 @@
         <v>9.6346388888888884E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -4623,7 +4638,7 @@
         <v>8.441111111111111E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -4640,7 +4655,7 @@
         <v>8.5444444444444446E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -4657,7 +4672,7 @@
         <v>1.0994291666666669</v>
       </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -4674,7 +4689,7 @@
         <v>1.110416666666667E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -4823,7 +4838,7 @@
         <v>14.15372472222222</v>
       </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>99</v>
       </c>
@@ -4990,7 +5005,7 @@
         <v>22.03856694444444</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>100</v>
       </c>
@@ -5154,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -5237,7 +5252,7 @@
         <v>102.187445</v>
       </c>
     </row>
-    <row r="31" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -5269,7 +5284,7 @@
         <v>100.56997</v>
       </c>
     </row>
-    <row r="32" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -5349,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -5429,7 +5444,7 @@
         <v>1.617475</v>
       </c>
     </row>
-    <row r="34" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -5515,7 +5530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -5547,7 +5562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -5633,7 +5648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -5797,7 +5812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -5904,7 +5919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -5978,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>111</v>
       </c>
@@ -6094,7 +6109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -6123,7 +6138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>113</v>
       </c>
@@ -6155,7 +6170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>114</v>
       </c>
@@ -6172,7 +6187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>115</v>
       </c>
@@ -6363,7 +6378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -6512,7 +6527,7 @@
         <v>148.8245541666667</v>
       </c>
     </row>
-    <row r="46" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -6532,7 +6547,7 @@
         <v>26.345791944444439</v>
       </c>
     </row>
-    <row r="47" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -6549,7 +6564,7 @@
         <v>10.30598472222222</v>
       </c>
     </row>
-    <row r="48" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>119</v>
       </c>
@@ -6569,7 +6584,7 @@
         <v>7.0122183333333332</v>
       </c>
     </row>
-    <row r="49" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>120</v>
       </c>
@@ -6586,7 +6601,7 @@
         <v>5.0237213888888892</v>
       </c>
     </row>
-    <row r="50" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>121</v>
       </c>
@@ -6603,7 +6618,7 @@
         <v>0.81025111111111114</v>
       </c>
     </row>
-    <row r="51" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -6623,7 +6638,7 @@
         <v>2.2792613888888891</v>
       </c>
     </row>
-    <row r="52" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>123</v>
       </c>
@@ -6640,7 +6655,7 @@
         <v>5.4600277777777782E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -6657,7 +6672,7 @@
         <v>8.4642500000000009E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>125</v>
       </c>
@@ -6674,7 +6689,7 @@
         <v>2.0252777777777782E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -6691,7 +6706,7 @@
         <v>0.75960944444444445</v>
       </c>
     </row>
-    <row r="56" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -6711,7 +6726,7 @@
         <v>1.347722222222222E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>128</v>
       </c>
@@ -6740,7 +6755,7 @@
         <v>13.464960833333331</v>
       </c>
     </row>
-    <row r="58" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>129</v>
       </c>
@@ -6766,7 +6781,7 @@
         <v>9.4671699999999994</v>
       </c>
     </row>
-    <row r="59" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>130</v>
       </c>
@@ -6792,7 +6807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>131</v>
       </c>
@@ -6887,7 +6902,7 @@
         <v>99.424285277777784</v>
       </c>
     </row>
-    <row r="61" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>132</v>
       </c>
@@ -6955,7 +6970,7 @@
         <v>97.809048333333337</v>
       </c>
     </row>
-    <row r="62" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -6975,7 +6990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>134</v>
       </c>
@@ -6995,7 +7010,7 @@
         <v>1.615236944444445</v>
       </c>
     </row>
-    <row r="64" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -7081,7 +7096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>136</v>
       </c>
@@ -7155,7 +7170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>137</v>
       </c>
@@ -7235,7 +7250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>138</v>
       </c>
@@ -7255,7 +7270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>139</v>
       </c>
@@ -7281,7 +7296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>140</v>
       </c>
@@ -7304,7 +7319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>141</v>
       </c>
@@ -7321,7 +7336,7 @@
         <v>0.1223461111111111</v>
       </c>
     </row>
-    <row r="71" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>142</v>
       </c>
@@ -7347,7 +7362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>143</v>
       </c>
@@ -7367,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -7390,7 +7405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>145</v>
       </c>
@@ -7452,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -7655,7 +7670,7 @@
         <v>12.24633527777778</v>
       </c>
     </row>
-    <row r="76" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>147</v>
       </c>
@@ -7849,7 +7864,7 @@
         <v>0.53495499999999996</v>
       </c>
     </row>
-    <row r="77" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>148</v>
       </c>
@@ -8043,7 +8058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>149</v>
       </c>
@@ -8138,7 +8153,7 @@
         <v>0.9428077777777778</v>
       </c>
     </row>
-    <row r="79" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>150</v>
       </c>
@@ -8260,7 +8275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>151</v>
       </c>
@@ -8454,7 +8469,7 @@
         <v>1.368264722222222</v>
       </c>
     </row>
-    <row r="81" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>152</v>
       </c>
@@ -8576,7 +8591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>153</v>
       </c>
@@ -8770,7 +8785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>154</v>
       </c>
@@ -8964,7 +8979,7 @@
         <v>4.9667955555555556</v>
       </c>
     </row>
-    <row r="84" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>155</v>
       </c>
@@ -9152,7 +9167,7 @@
         <v>4.4335119444444446</v>
       </c>
     </row>
-    <row r="85" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>156</v>
       </c>
@@ -9172,7 +9187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>157</v>
       </c>
@@ -9252,7 +9267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>158</v>
       </c>
@@ -9275,7 +9290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>159</v>
       </c>
@@ -9337,7 +9352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>160</v>
       </c>
@@ -9360,7 +9375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>161</v>
       </c>
@@ -9422,7 +9437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>162</v>
       </c>
@@ -9616,7 +9631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>163</v>
       </c>
@@ -9810,7 +9825,7 @@
         <v>2.6267841666666669</v>
       </c>
     </row>
-    <row r="93" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>164</v>
       </c>
@@ -10030,8 +10045,20 @@
       <c r="BU93">
         <v>216.58698666666669</v>
       </c>
+      <c r="BV93">
+        <f>BR93+X93+C93+W93+BS93+BM93+AU93+N93</f>
+        <v>331.73826194444445</v>
+      </c>
+      <c r="BW93">
+        <f>BR93+BS93+BT93+BU93</f>
+        <v>363.11410333333333</v>
+      </c>
+      <c r="BY93">
+        <f>BC93+BD93+BF93+BG93+BH93+BL93</f>
+        <v>45.01538305555556</v>
+      </c>
     </row>
-    <row r="94" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>165</v>
       </c>
@@ -10180,7 +10207,7 @@
         <v>24.71958305555555</v>
       </c>
     </row>
-    <row r="95" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>166</v>
       </c>
@@ -10329,7 +10356,7 @@
         <v>24.479941388888889</v>
       </c>
     </row>
-    <row r="96" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>167</v>
       </c>
@@ -10415,7 +10442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>168</v>
       </c>
@@ -10501,7 +10528,7 @@
         <v>6.4325555555555552E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>169</v>
       </c>
@@ -10590,7 +10617,7 @@
         <v>24.205071944444441</v>
       </c>
     </row>
-    <row r="99" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>170</v>
       </c>
@@ -10739,7 +10766,7 @@
         <v>0.22545305555555559</v>
       </c>
     </row>
-    <row r="100" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>171</v>
       </c>
@@ -10888,7 +10915,7 @@
         <v>1.418888888888889E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>172</v>
       </c>
@@ -11084,8 +11111,16 @@
       <c r="BU101">
         <v>191.8604402777778</v>
       </c>
+      <c r="BV101">
+        <f t="shared" ref="BV94:BV102" si="0">BR101+X101+C101+W101+BS101+BM101+AU101+N101</f>
+        <v>306.99272861111115</v>
+      </c>
+      <c r="BW101">
+        <f t="shared" ref="BW94:BW101" si="1">BR101+BS101+BT101+BU101</f>
+        <v>338.41493666666668</v>
+      </c>
     </row>
-    <row r="102" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>173</v>
       </c>
@@ -11281,8 +11316,12 @@
       <c r="BU102">
         <v>50.345647777777778</v>
       </c>
+      <c r="BV102">
+        <f t="shared" si="0"/>
+        <v>88.466093888888906</v>
+      </c>
     </row>
-    <row r="103" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>174</v>
       </c>
@@ -11476,7 +11515,7 @@
         <v>8.1047597222222212</v>
       </c>
     </row>
-    <row r="104" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>175</v>
       </c>
@@ -11670,7 +11709,7 @@
         <v>8.1078036111111107</v>
       </c>
     </row>
-    <row r="105" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>176</v>
       </c>
@@ -11864,7 +11903,7 @@
         <v>1.672666666666667</v>
       </c>
     </row>
-    <row r="106" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>177</v>
       </c>
@@ -12058,7 +12097,7 @@
         <v>8.8930600000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>178</v>
       </c>
@@ -12252,7 +12291,7 @@
         <v>0.80253555555555556</v>
       </c>
     </row>
-    <row r="108" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>179</v>
       </c>
@@ -12446,7 +12485,7 @@
         <v>3.0318930555555559</v>
       </c>
     </row>
-    <row r="109" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>180</v>
       </c>
@@ -12640,7 +12679,7 @@
         <v>1.406973333333333</v>
       </c>
     </row>
-    <row r="110" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>181</v>
       </c>
@@ -12834,7 +12873,7 @@
         <v>4.3947016666666663</v>
       </c>
     </row>
-    <row r="111" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>182</v>
       </c>
@@ -13028,7 +13067,7 @@
         <v>8.1537730555555559</v>
       </c>
     </row>
-    <row r="112" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>183</v>
       </c>
@@ -13222,7 +13261,7 @@
         <v>1.645030833333333</v>
       </c>
     </row>
-    <row r="113" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>184</v>
       </c>
@@ -13416,7 +13455,7 @@
         <v>2.677175833333334</v>
       </c>
     </row>
-    <row r="114" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>185</v>
       </c>
@@ -13610,7 +13649,7 @@
         <v>0.50618833333333335</v>
       </c>
     </row>
-    <row r="115" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>186</v>
       </c>
@@ -13804,7 +13843,7 @@
         <v>0.9490858333333333</v>
       </c>
     </row>
-    <row r="116" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>187</v>
       </c>
@@ -13995,7 +14034,7 @@
         <v>84.845475833333325</v>
       </c>
     </row>
-    <row r="117" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>188</v>
       </c>
@@ -14183,7 +14222,7 @@
         <v>0.69652027777777781</v>
       </c>
     </row>
-    <row r="118" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>189</v>
       </c>
@@ -14314,7 +14353,7 @@
         <v>81.467903888888898</v>
       </c>
     </row>
-    <row r="119" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>190</v>
       </c>
@@ -14400,7 +14439,7 @@
         <v>0.19077472222222219</v>
       </c>
     </row>
-    <row r="120" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>191</v>
       </c>
@@ -14585,7 +14624,7 @@
         <v>0.35615833333333341</v>
       </c>
     </row>
-    <row r="121" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>192</v>
       </c>
@@ -14677,7 +14716,7 @@
         <v>1.9059663888888889</v>
       </c>
     </row>
-    <row r="122" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>193</v>
       </c>
@@ -14868,7 +14907,7 @@
         <v>0.22815277777777779</v>
       </c>
     </row>
-    <row r="123" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>194</v>
       </c>
@@ -15065,7 +15104,7 @@
         <v>56.669316388888888</v>
       </c>
     </row>
-    <row r="124" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>195</v>
       </c>
@@ -15262,7 +15301,7 @@
         <v>13.208240555555561</v>
       </c>
     </row>
-    <row r="125" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>196</v>
       </c>
@@ -15459,7 +15498,7 @@
         <v>40.304588333333342</v>
       </c>
     </row>
-    <row r="126" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>197</v>
       </c>
@@ -15653,7 +15692,7 @@
         <v>3.1564874999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>198</v>
       </c>
@@ -15847,7 +15886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>199</v>
       </c>
@@ -16044,7 +16083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>200</v>
       </c>
@@ -16259,7 +16298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>201</v>
       </c>
@@ -16426,7 +16465,7 @@
         <v>14.18388527777778</v>
       </c>
     </row>
-    <row r="131" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>202</v>
       </c>
@@ -16593,7 +16632,7 @@
         <v>2.4754166666666668</v>
       </c>
     </row>
-    <row r="132" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>203</v>
       </c>
@@ -16748,7 +16787,7 @@
         <v>6.6080258333333326</v>
       </c>
     </row>
-    <row r="133" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>204</v>
       </c>
@@ -16915,7 +16954,7 @@
         <v>3.2021747222222219</v>
       </c>
     </row>
-    <row r="134" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>205</v>
       </c>
@@ -17070,7 +17109,7 @@
         <v>1.898268055555556</v>
       </c>
     </row>
-    <row r="135" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>206</v>
       </c>
@@ -17231,7 +17270,7 @@
         <v>12.14842916666667</v>
       </c>
     </row>
-    <row r="136" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>207</v>
       </c>
@@ -17392,7 +17431,7 @@
         <v>7.6432616666666666</v>
       </c>
     </row>
-    <row r="137" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>208</v>
       </c>
@@ -17553,7 +17592,7 @@
         <v>2.578554722222222</v>
       </c>
     </row>
-    <row r="138" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>209</v>
       </c>
@@ -17714,7 +17753,7 @@
         <v>1.8630827777777781</v>
       </c>
     </row>
-    <row r="139" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:73" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>210</v>
       </c>

</xml_diff>

<commit_message>
refactored site, extended plotting
</commit_message>
<xml_diff>
--- a/data/data_raw/eurostat/AT_2021_energy_balance_TWh.xlsx
+++ b/data/data_raw/eurostat/AT_2021_energy_balance_TWh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernhard\Documents\EnergyAnalysis\Data\Dashboard\data\data_raw\eurostat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF28715-BF31-4138-990E-410651ECE3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEDFAD8-F2F8-45C7-A0B2-4D025A26553F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,10 +1036,10 @@
   <dimension ref="A1:BY139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BL88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BO78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BT96" sqref="BT96"/>
+      <selection pane="bottomRight" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11112,11 +11112,11 @@
         <v>191.8604402777778</v>
       </c>
       <c r="BV101">
-        <f t="shared" ref="BV94:BV102" si="0">BR101+X101+C101+W101+BS101+BM101+AU101+N101</f>
+        <f t="shared" ref="BV101:BV102" si="0">BR101+X101+C101+W101+BS101+BM101+AU101+N101</f>
         <v>306.99272861111115</v>
       </c>
       <c r="BW101">
-        <f t="shared" ref="BW94:BW101" si="1">BR101+BS101+BT101+BU101</f>
+        <f t="shared" ref="BW101" si="1">BR101+BS101+BT101+BU101</f>
         <v>338.41493666666668</v>
       </c>
     </row>

</xml_diff>